<commit_message>
Fixes #1, Code concept change
notify long time create db on first run, set edittext attribute in
fragment class
</commit_message>
<xml_diff>
--- a/01-設計書/チェックリスト.xlsx
+++ b/01-設計書/チェックリスト.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LSI\Documents\project\Android_study\kanji_decompose\設計書\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LSI\Documents\GitHub\kanji-decomposition\01-設計書\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>項目</t>
   </si>
@@ -73,6 +73,24 @@
     <t>画面作成</t>
     <rPh sb="0" eb="4">
       <t>ガメンサクセイ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>アプリピーアール</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>済</t>
+    <rPh sb="0" eb="1">
+      <t>スミ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>調べている</t>
+    <rPh sb="0" eb="1">
+      <t>シラ</t>
     </rPh>
     <phoneticPr fontId="18"/>
   </si>
@@ -1124,7 +1142,7 @@
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1160,11 +1178,17 @@
       <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="8"/>

</xml_diff>

<commit_message>
This should closes #3 #4 #7
If problem arises then open again
</commit_message>
<xml_diff>
--- a/01-設計書/チェックリスト.xlsx
+++ b/01-設計書/チェックリスト.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LSI\Documents\GitHub\kanji-decomposition\01-設計書\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16296" windowHeight="3984"/>
   </bookViews>
@@ -24,7 +19,7 @@
     <author>LSI</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>項目</t>
   </si>
@@ -77,10 +72,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>アプリピーアール</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>済</t>
     <rPh sb="0" eb="1">
       <t>スミ</t>
@@ -94,6 +85,32 @@
     </rPh>
     <phoneticPr fontId="18"/>
   </si>
+  <si>
+    <t>勉強課題</t>
+    <rPh sb="0" eb="4">
+      <t>ベンキョウカダイ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>AdapterView</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>待ってる</t>
+    <rPh sb="0" eb="1">
+      <t>マ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>アプリピーアール
+＊ GooglePlayで公開する</t>
+    <rPh sb="22" eb="24">
+      <t>コウカイ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
 </sst>
 </file>
 
@@ -438,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -661,6 +678,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -790,7 +893,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -817,6 +920,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -919,7 +1043,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -954,7 +1078,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1131,7 +1255,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1139,70 +1263,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.44140625" customWidth="1"/>
     <col min="3" max="3" width="4.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="F4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>2</v>
       </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="2:7" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="2:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="6"/>
     </row>

</xml_diff>